<commit_message>
Integrate WS with Angular part.
</commit_message>
<xml_diff>
--- a/Docs/CarsPlan.xlsx
+++ b/Docs/CarsPlan.xlsx
@@ -24,7 +24,7 @@
     <definedName name="vertex42_id" hidden="1">"gantt-chart_L.xlsx"</definedName>
     <definedName name="vertex42_title" hidden="1">"Gantt Chart Template"</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">GanttChart!$4:$7</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">GanttChart!$A$1:$BN$30</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">GanttChart!$A$1:$BN$32</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">GanttChartPro!$A$1:$C$47</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -442,7 +442,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="160">
   <si>
     <t>WBS</t>
   </si>
@@ -1575,6 +1575,12 @@
   <si>
     <t xml:space="preserve"> . . Create Web Service Controller</t>
   </si>
+  <si>
+    <t xml:space="preserve"> . . . Del static data from Razor view</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> . . . Consume WS data in Repo</t>
+  </si>
 </sst>
 </file>
 
@@ -1585,7 +1591,7 @@
     <numFmt numFmtId="165" formatCode="d"/>
     <numFmt numFmtId="166" formatCode="d\ mmm\ yyyy"/>
   </numFmts>
-  <fonts count="74" x14ac:knownFonts="1">
+  <fonts count="77" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2060,10 +2066,31 @@
       <b/>
       <i/>
       <sz val="9"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF0070C0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF0070C0"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -2541,7 +2568,7 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="159">
+  <cellXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
@@ -2935,6 +2962,15 @@
     </xf>
     <xf numFmtId="0" fontId="73" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -2983,7 +3019,7 @@
     <cellStyle name="Текст предупреждения" xfId="43" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Хороший" xfId="29" builtinId="26" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="76">
+  <dxfs count="88">
     <dxf>
       <border>
         <left style="thin">
@@ -3583,12 +3619,116 @@
       </fill>
     </dxf>
     <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color theme="0"/>
       </font>
       <fill>
         <patternFill>
           <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4388,11 +4528,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BN37"/>
+  <dimension ref="A1:BN39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
+      <pane ySplit="7" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5281,7 +5421,7 @@
         <v>0.5</v>
       </c>
       <c r="I9" s="82">
-        <f t="shared" ref="I9:I30" si="5">IF(OR(F9=0,E9=0)," - ",NETWORKDAYS(E9,F9))</f>
+        <f t="shared" ref="I9:I32" si="5">IF(OR(F9=0,E9=0)," - ",NETWORKDAYS(E9,F9))</f>
         <v>3</v>
       </c>
       <c r="J9" s="85"/>
@@ -5514,7 +5654,7 @@
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>2.2.1</v>
       </c>
-      <c r="B12" s="74" t="s">
+      <c r="B12" s="161" t="s">
         <v>153</v>
       </c>
       <c r="C12" s="73"/>
@@ -5595,7 +5735,7 @@
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>2.2.2</v>
       </c>
-      <c r="B13" s="74" t="s">
+      <c r="B13" s="161" t="s">
         <v>154</v>
       </c>
       <c r="C13" s="73"/>
@@ -5772,7 +5912,7 @@
         <v>2</v>
       </c>
       <c r="H15" s="56">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="I15" s="72">
         <f>IF(OR(F15=0,E15=0)," - ",NETWORKDAYS(E15,F15))</f>
@@ -5851,7 +5991,7 @@
         <v>43566</v>
       </c>
       <c r="F16" s="145">
-        <f t="shared" ref="F16:F28" si="7">IF(ISBLANK(E16)," - ",IF(G16=0,E16,E16+G16-1))</f>
+        <f t="shared" ref="F16:F30" si="7">IF(ISBLANK(E16)," - ",IF(G16=0,E16,E16+G16-1))</f>
         <v>43566</v>
       </c>
       <c r="G16" s="55">
@@ -5861,7 +6001,7 @@
         <v>1</v>
       </c>
       <c r="I16" s="72">
-        <f t="shared" ref="I16:I28" si="8">IF(OR(F16=0,E16=0)," - ",NETWORKDAYS(E16,F16))</f>
+        <f t="shared" ref="I16:I30" si="8">IF(OR(F16=0,E16=0)," - ",NETWORKDAYS(E16,F16))</f>
         <v>1</v>
       </c>
       <c r="J16" s="88"/>
@@ -5927,7 +6067,7 @@
         <f t="shared" ref="A17:A23" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>3.1.1</v>
       </c>
-      <c r="B17" s="74" t="s">
+      <c r="B17" s="161" t="s">
         <v>146</v>
       </c>
       <c r="C17" s="73"/>
@@ -6008,7 +6148,7 @@
         <f t="shared" si="9"/>
         <v>3.1.2</v>
       </c>
-      <c r="B18" s="74" t="s">
+      <c r="B18" s="161" t="s">
         <v>145</v>
       </c>
       <c r="C18" s="73"/>
@@ -6089,7 +6229,7 @@
         <f t="shared" si="9"/>
         <v>3.1.3</v>
       </c>
-      <c r="B19" s="74" t="s">
+      <c r="B19" s="161" t="s">
         <v>147</v>
       </c>
       <c r="C19" s="73"/>
@@ -6170,7 +6310,7 @@
         <f t="shared" si="9"/>
         <v>3.1.4</v>
       </c>
-      <c r="B20" s="74" t="s">
+      <c r="B20" s="161" t="s">
         <v>148</v>
       </c>
       <c r="C20" s="73"/>
@@ -6251,7 +6391,7 @@
         <f t="shared" si="9"/>
         <v>3.1.5</v>
       </c>
-      <c r="B21" s="74" t="s">
+      <c r="B21" s="161" t="s">
         <v>149</v>
       </c>
       <c r="C21" s="73"/>
@@ -6332,7 +6472,7 @@
         <f t="shared" si="9"/>
         <v>3.1.6</v>
       </c>
-      <c r="B22" s="74" t="s">
+      <c r="B22" s="161" t="s">
         <v>150</v>
       </c>
       <c r="C22" s="73"/>
@@ -6413,7 +6553,7 @@
         <f t="shared" si="9"/>
         <v>3.1.7</v>
       </c>
-      <c r="B23" s="74" t="s">
+      <c r="B23" s="161" t="s">
         <v>151</v>
       </c>
       <c r="C23" s="73"/>
@@ -6677,7 +6817,9 @@
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G26" s="55"/>
-      <c r="H26" s="56"/>
+      <c r="H26" s="56">
+        <v>1</v>
+      </c>
       <c r="I26" s="72" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve"> - </v>
@@ -6745,7 +6887,7 @@
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>3.4.1</v>
       </c>
-      <c r="B27" s="74" t="s">
+      <c r="B27" s="159" t="s">
         <v>157</v>
       </c>
       <c r="C27" s="73"/>
@@ -6756,7 +6898,9 @@
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G27" s="55"/>
-      <c r="H27" s="56"/>
+      <c r="H27" s="56">
+        <v>1</v>
+      </c>
       <c r="I27" s="72" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve"> - </v>
@@ -6824,7 +6968,7 @@
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>3.4.2</v>
       </c>
-      <c r="B28" s="74" t="s">
+      <c r="B28" s="159" t="s">
         <v>156</v>
       </c>
       <c r="C28" s="73"/>
@@ -6835,7 +6979,9 @@
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G28" s="55"/>
-      <c r="H28" s="56"/>
+      <c r="H28" s="56">
+        <v>1</v>
+      </c>
       <c r="I28" s="72" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve"> - </v>
@@ -6899,15 +7045,28 @@
       <c r="BN28" s="93"/>
     </row>
     <row r="29" spans="1:66" s="62" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A29" s="110"/>
-      <c r="B29" s="111"/>
-      <c r="C29" s="70"/>
+      <c r="A29" s="54" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",4))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",3))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",4))-FIND("`",SUBSTITUTE(prevWBS,".","`",3))-1)))+1)))</f>
+        <v>3.4.2.1</v>
+      </c>
+      <c r="B29" s="160" t="s">
+        <v>158</v>
+      </c>
+      <c r="C29" s="73"/>
       <c r="D29" s="71"/>
       <c r="E29" s="144"/>
-      <c r="F29" s="145"/>
+      <c r="F29" s="145" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve"> - </v>
+      </c>
       <c r="G29" s="55"/>
-      <c r="H29" s="56"/>
-      <c r="I29" s="72"/>
+      <c r="H29" s="56">
+        <v>1</v>
+      </c>
+      <c r="I29" s="72" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve"> - </v>
+      </c>
       <c r="J29" s="88"/>
       <c r="K29" s="93"/>
       <c r="L29" s="93"/>
@@ -6967,19 +7126,29 @@
       <c r="BN29" s="93"/>
     </row>
     <row r="30" spans="1:66" s="62" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A30" s="54"/>
-      <c r="B30" s="57"/>
-      <c r="C30" s="57"/>
-      <c r="D30" s="58"/>
-      <c r="E30" s="89"/>
-      <c r="F30" s="89"/>
-      <c r="G30" s="59"/>
-      <c r="H30" s="60"/>
-      <c r="I30" s="61" t="str">
-        <f t="shared" si="5"/>
+      <c r="A30" s="54" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",4))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",3))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",4))-FIND("`",SUBSTITUTE(prevWBS,".","`",3))-1)))+1)))</f>
+        <v>3.4.2.2</v>
+      </c>
+      <c r="B30" s="160" t="s">
+        <v>159</v>
+      </c>
+      <c r="C30" s="73"/>
+      <c r="D30" s="71"/>
+      <c r="E30" s="144"/>
+      <c r="F30" s="145" t="str">
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="J30" s="86"/>
+      <c r="G30" s="55"/>
+      <c r="H30" s="56">
+        <v>1</v>
+      </c>
+      <c r="I30" s="72" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J30" s="88"/>
       <c r="K30" s="93"/>
       <c r="L30" s="93"/>
       <c r="M30" s="93"/>
@@ -7037,19 +7206,17 @@
       <c r="BM30" s="93"/>
       <c r="BN30" s="93"/>
     </row>
-    <row r="31" spans="1:66" s="67" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A31" s="63" t="s">
-        <v>1</v>
-      </c>
-      <c r="B31" s="64"/>
-      <c r="C31" s="65"/>
-      <c r="D31" s="65"/>
-      <c r="E31" s="90"/>
-      <c r="F31" s="90"/>
-      <c r="G31" s="66"/>
-      <c r="H31" s="66"/>
-      <c r="I31" s="66"/>
-      <c r="J31" s="87"/>
+    <row r="31" spans="1:66" s="62" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A31" s="110"/>
+      <c r="B31" s="111"/>
+      <c r="C31" s="70"/>
+      <c r="D31" s="71"/>
+      <c r="E31" s="144"/>
+      <c r="F31" s="145"/>
+      <c r="G31" s="55"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="72"/>
+      <c r="J31" s="88"/>
       <c r="K31" s="93"/>
       <c r="L31" s="93"/>
       <c r="M31" s="93"/>
@@ -7108,18 +7275,19 @@
       <c r="BN31" s="93"/>
     </row>
     <row r="32" spans="1:66" s="62" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A32" s="68" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" s="69"/>
-      <c r="C32" s="69"/>
-      <c r="D32" s="69"/>
-      <c r="E32" s="91"/>
-      <c r="F32" s="91"/>
-      <c r="G32" s="69"/>
-      <c r="H32" s="69"/>
-      <c r="I32" s="69"/>
-      <c r="J32" s="87"/>
+      <c r="A32" s="54"/>
+      <c r="B32" s="57"/>
+      <c r="C32" s="57"/>
+      <c r="D32" s="58"/>
+      <c r="E32" s="89"/>
+      <c r="F32" s="89"/>
+      <c r="G32" s="59"/>
+      <c r="H32" s="60"/>
+      <c r="I32" s="61" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J32" s="86"/>
       <c r="K32" s="93"/>
       <c r="L32" s="93"/>
       <c r="M32" s="93"/>
@@ -7177,28 +7345,19 @@
       <c r="BM32" s="93"/>
       <c r="BN32" s="93"/>
     </row>
-    <row r="33" spans="1:66" s="62" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A33" s="110" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+    <row r="33" spans="1:66" s="67" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A33" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B33" s="111" t="s">
-        <v>76</v>
-      </c>
-      <c r="C33" s="70"/>
-      <c r="D33" s="71"/>
-      <c r="E33" s="144"/>
-      <c r="F33" s="145" t="str">
-        <f t="shared" ref="F33:F36" si="10">IF(ISBLANK(E33)," - ",IF(G33=0,E33,E33+G33-1))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G33" s="55"/>
-      <c r="H33" s="56"/>
-      <c r="I33" s="72" t="str">
-        <f>IF(OR(F33=0,E33=0)," - ",NETWORKDAYS(E33,F33))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J33" s="88"/>
+      <c r="B33" s="64"/>
+      <c r="C33" s="65"/>
+      <c r="D33" s="65"/>
+      <c r="E33" s="90"/>
+      <c r="F33" s="90"/>
+      <c r="G33" s="66"/>
+      <c r="H33" s="66"/>
+      <c r="I33" s="66"/>
+      <c r="J33" s="87"/>
       <c r="K33" s="93"/>
       <c r="L33" s="93"/>
       <c r="M33" s="93"/>
@@ -7257,27 +7416,18 @@
       <c r="BN33" s="93"/>
     </row>
     <row r="34" spans="1:66" s="62" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A34" s="54" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>1.1</v>
-      </c>
-      <c r="B34" s="147" t="s">
-        <v>62</v>
-      </c>
-      <c r="C34" s="73"/>
-      <c r="D34" s="71"/>
-      <c r="E34" s="144"/>
-      <c r="F34" s="145" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G34" s="55"/>
-      <c r="H34" s="56"/>
-      <c r="I34" s="72" t="str">
-        <f t="shared" ref="I34:I36" si="11">IF(OR(F34=0,E34=0)," - ",NETWORKDAYS(E34,F34))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J34" s="88"/>
+      <c r="A34" s="68" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="69"/>
+      <c r="C34" s="69"/>
+      <c r="D34" s="69"/>
+      <c r="E34" s="91"/>
+      <c r="F34" s="91"/>
+      <c r="G34" s="69"/>
+      <c r="H34" s="69"/>
+      <c r="I34" s="69"/>
+      <c r="J34" s="87"/>
       <c r="K34" s="93"/>
       <c r="L34" s="93"/>
       <c r="M34" s="93"/>
@@ -7336,24 +7486,24 @@
       <c r="BN34" s="93"/>
     </row>
     <row r="35" spans="1:66" s="62" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A35" s="54" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
-        <v>1.1.1</v>
-      </c>
-      <c r="B35" s="74" t="s">
-        <v>63</v>
-      </c>
-      <c r="C35" s="73"/>
+      <c r="A35" s="110" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>1</v>
+      </c>
+      <c r="B35" s="111" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" s="70"/>
       <c r="D35" s="71"/>
       <c r="E35" s="144"/>
       <c r="F35" s="145" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="F35:F38" si="10">IF(ISBLANK(E35)," - ",IF(G35=0,E35,E35+G35-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G35" s="55"/>
       <c r="H35" s="56"/>
       <c r="I35" s="72" t="str">
-        <f t="shared" si="11"/>
+        <f>IF(OR(F35=0,E35=0)," - ",NETWORKDAYS(E35,F35))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J35" s="88"/>
@@ -7416,11 +7566,11 @@
     </row>
     <row r="36" spans="1:66" s="62" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A36" s="54" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",4))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",3))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",4))-FIND("`",SUBSTITUTE(prevWBS,".","`",3))-1)))+1)))</f>
-        <v>1.1.1.1</v>
-      </c>
-      <c r="B36" s="74" t="s">
-        <v>64</v>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>1.1</v>
+      </c>
+      <c r="B36" s="147" t="s">
+        <v>62</v>
       </c>
       <c r="C36" s="73"/>
       <c r="D36" s="71"/>
@@ -7432,7 +7582,7 @@
       <c r="G36" s="55"/>
       <c r="H36" s="56"/>
       <c r="I36" s="72" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="I36:I38" si="11">IF(OR(F36=0,E36=0)," - ",NETWORKDAYS(E36,F36))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J36" s="88"/>
@@ -7493,73 +7643,231 @@
       <c r="BM36" s="93"/>
       <c r="BN36" s="93"/>
     </row>
-    <row r="37" spans="1:66" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="30"/>
-      <c r="B37" s="31"/>
-      <c r="C37" s="31"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
-      <c r="G37" s="31"/>
-      <c r="H37" s="31"/>
-      <c r="I37" s="31"/>
-      <c r="J37" s="31"/>
-      <c r="K37" s="31"/>
-      <c r="L37" s="31"/>
-      <c r="M37" s="31"/>
-      <c r="N37" s="31"/>
-      <c r="O37" s="31"/>
-      <c r="P37" s="31"/>
-      <c r="Q37" s="31"/>
-      <c r="R37" s="31"/>
-      <c r="S37" s="31"/>
-      <c r="T37" s="31"/>
-      <c r="U37" s="31"/>
-      <c r="V37" s="31"/>
-      <c r="W37" s="31"/>
-      <c r="X37" s="31"/>
-      <c r="Y37" s="31"/>
-      <c r="Z37" s="31"/>
-      <c r="AA37" s="31"/>
-      <c r="AB37" s="31"/>
-      <c r="AC37" s="31"/>
-      <c r="AD37" s="31"/>
-      <c r="AE37" s="31"/>
-      <c r="AF37" s="31"/>
-      <c r="AG37" s="31"/>
-      <c r="AH37" s="31"/>
-      <c r="AI37" s="31"/>
-      <c r="AJ37" s="31"/>
-      <c r="AK37" s="31"/>
-      <c r="AL37" s="31"/>
-      <c r="AM37" s="31"/>
-      <c r="AN37" s="31"/>
-      <c r="AO37" s="31"/>
-      <c r="AP37" s="31"/>
-      <c r="AQ37" s="31"/>
-      <c r="AR37" s="31"/>
-      <c r="AS37" s="31"/>
-      <c r="AT37" s="31"/>
-      <c r="AU37" s="31"/>
-      <c r="AV37" s="31"/>
-      <c r="AW37" s="31"/>
-      <c r="AX37" s="31"/>
-      <c r="AY37" s="31"/>
-      <c r="AZ37" s="31"/>
-      <c r="BA37" s="31"/>
-      <c r="BB37" s="31"/>
-      <c r="BC37" s="31"/>
-      <c r="BD37" s="31"/>
-      <c r="BE37" s="31"/>
-      <c r="BF37" s="31"/>
-      <c r="BG37" s="31"/>
-      <c r="BH37" s="31"/>
-      <c r="BI37" s="31"/>
-      <c r="BJ37" s="31"/>
-      <c r="BK37" s="31"/>
-      <c r="BL37" s="31"/>
-      <c r="BM37" s="31"/>
-      <c r="BN37" s="31"/>
+    <row r="37" spans="1:66" s="62" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A37" s="54" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
+        <v>1.1.1</v>
+      </c>
+      <c r="B37" s="74" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" s="73"/>
+      <c r="D37" s="71"/>
+      <c r="E37" s="144"/>
+      <c r="F37" s="145" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G37" s="55"/>
+      <c r="H37" s="56"/>
+      <c r="I37" s="72" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J37" s="88"/>
+      <c r="K37" s="93"/>
+      <c r="L37" s="93"/>
+      <c r="M37" s="93"/>
+      <c r="N37" s="93"/>
+      <c r="O37" s="93"/>
+      <c r="P37" s="93"/>
+      <c r="Q37" s="93"/>
+      <c r="R37" s="93"/>
+      <c r="S37" s="93"/>
+      <c r="T37" s="93"/>
+      <c r="U37" s="93"/>
+      <c r="V37" s="93"/>
+      <c r="W37" s="93"/>
+      <c r="X37" s="93"/>
+      <c r="Y37" s="93"/>
+      <c r="Z37" s="93"/>
+      <c r="AA37" s="93"/>
+      <c r="AB37" s="93"/>
+      <c r="AC37" s="93"/>
+      <c r="AD37" s="93"/>
+      <c r="AE37" s="93"/>
+      <c r="AF37" s="93"/>
+      <c r="AG37" s="93"/>
+      <c r="AH37" s="93"/>
+      <c r="AI37" s="93"/>
+      <c r="AJ37" s="93"/>
+      <c r="AK37" s="93"/>
+      <c r="AL37" s="93"/>
+      <c r="AM37" s="93"/>
+      <c r="AN37" s="93"/>
+      <c r="AO37" s="93"/>
+      <c r="AP37" s="93"/>
+      <c r="AQ37" s="93"/>
+      <c r="AR37" s="93"/>
+      <c r="AS37" s="93"/>
+      <c r="AT37" s="93"/>
+      <c r="AU37" s="93"/>
+      <c r="AV37" s="93"/>
+      <c r="AW37" s="93"/>
+      <c r="AX37" s="93"/>
+      <c r="AY37" s="93"/>
+      <c r="AZ37" s="93"/>
+      <c r="BA37" s="93"/>
+      <c r="BB37" s="93"/>
+      <c r="BC37" s="93"/>
+      <c r="BD37" s="93"/>
+      <c r="BE37" s="93"/>
+      <c r="BF37" s="93"/>
+      <c r="BG37" s="93"/>
+      <c r="BH37" s="93"/>
+      <c r="BI37" s="93"/>
+      <c r="BJ37" s="93"/>
+      <c r="BK37" s="93"/>
+      <c r="BL37" s="93"/>
+      <c r="BM37" s="93"/>
+      <c r="BN37" s="93"/>
+    </row>
+    <row r="38" spans="1:66" s="62" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A38" s="54" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",4))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",3))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",4))-FIND("`",SUBSTITUTE(prevWBS,".","`",3))-1)))+1)))</f>
+        <v>1.1.1.1</v>
+      </c>
+      <c r="B38" s="74" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38" s="73"/>
+      <c r="D38" s="71"/>
+      <c r="E38" s="144"/>
+      <c r="F38" s="145" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G38" s="55"/>
+      <c r="H38" s="56"/>
+      <c r="I38" s="72" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J38" s="88"/>
+      <c r="K38" s="93"/>
+      <c r="L38" s="93"/>
+      <c r="M38" s="93"/>
+      <c r="N38" s="93"/>
+      <c r="O38" s="93"/>
+      <c r="P38" s="93"/>
+      <c r="Q38" s="93"/>
+      <c r="R38" s="93"/>
+      <c r="S38" s="93"/>
+      <c r="T38" s="93"/>
+      <c r="U38" s="93"/>
+      <c r="V38" s="93"/>
+      <c r="W38" s="93"/>
+      <c r="X38" s="93"/>
+      <c r="Y38" s="93"/>
+      <c r="Z38" s="93"/>
+      <c r="AA38" s="93"/>
+      <c r="AB38" s="93"/>
+      <c r="AC38" s="93"/>
+      <c r="AD38" s="93"/>
+      <c r="AE38" s="93"/>
+      <c r="AF38" s="93"/>
+      <c r="AG38" s="93"/>
+      <c r="AH38" s="93"/>
+      <c r="AI38" s="93"/>
+      <c r="AJ38" s="93"/>
+      <c r="AK38" s="93"/>
+      <c r="AL38" s="93"/>
+      <c r="AM38" s="93"/>
+      <c r="AN38" s="93"/>
+      <c r="AO38" s="93"/>
+      <c r="AP38" s="93"/>
+      <c r="AQ38" s="93"/>
+      <c r="AR38" s="93"/>
+      <c r="AS38" s="93"/>
+      <c r="AT38" s="93"/>
+      <c r="AU38" s="93"/>
+      <c r="AV38" s="93"/>
+      <c r="AW38" s="93"/>
+      <c r="AX38" s="93"/>
+      <c r="AY38" s="93"/>
+      <c r="AZ38" s="93"/>
+      <c r="BA38" s="93"/>
+      <c r="BB38" s="93"/>
+      <c r="BC38" s="93"/>
+      <c r="BD38" s="93"/>
+      <c r="BE38" s="93"/>
+      <c r="BF38" s="93"/>
+      <c r="BG38" s="93"/>
+      <c r="BH38" s="93"/>
+      <c r="BI38" s="93"/>
+      <c r="BJ38" s="93"/>
+      <c r="BK38" s="93"/>
+      <c r="BL38" s="93"/>
+      <c r="BM38" s="93"/>
+      <c r="BN38" s="93"/>
+    </row>
+    <row r="39" spans="1:66" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="30"/>
+      <c r="B39" s="31"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="31"/>
+      <c r="H39" s="31"/>
+      <c r="I39" s="31"/>
+      <c r="J39" s="31"/>
+      <c r="K39" s="31"/>
+      <c r="L39" s="31"/>
+      <c r="M39" s="31"/>
+      <c r="N39" s="31"/>
+      <c r="O39" s="31"/>
+      <c r="P39" s="31"/>
+      <c r="Q39" s="31"/>
+      <c r="R39" s="31"/>
+      <c r="S39" s="31"/>
+      <c r="T39" s="31"/>
+      <c r="U39" s="31"/>
+      <c r="V39" s="31"/>
+      <c r="W39" s="31"/>
+      <c r="X39" s="31"/>
+      <c r="Y39" s="31"/>
+      <c r="Z39" s="31"/>
+      <c r="AA39" s="31"/>
+      <c r="AB39" s="31"/>
+      <c r="AC39" s="31"/>
+      <c r="AD39" s="31"/>
+      <c r="AE39" s="31"/>
+      <c r="AF39" s="31"/>
+      <c r="AG39" s="31"/>
+      <c r="AH39" s="31"/>
+      <c r="AI39" s="31"/>
+      <c r="AJ39" s="31"/>
+      <c r="AK39" s="31"/>
+      <c r="AL39" s="31"/>
+      <c r="AM39" s="31"/>
+      <c r="AN39" s="31"/>
+      <c r="AO39" s="31"/>
+      <c r="AP39" s="31"/>
+      <c r="AQ39" s="31"/>
+      <c r="AR39" s="31"/>
+      <c r="AS39" s="31"/>
+      <c r="AT39" s="31"/>
+      <c r="AU39" s="31"/>
+      <c r="AV39" s="31"/>
+      <c r="AW39" s="31"/>
+      <c r="AX39" s="31"/>
+      <c r="AY39" s="31"/>
+      <c r="AZ39" s="31"/>
+      <c r="BA39" s="31"/>
+      <c r="BB39" s="31"/>
+      <c r="BC39" s="31"/>
+      <c r="BD39" s="31"/>
+      <c r="BE39" s="31"/>
+      <c r="BF39" s="31"/>
+      <c r="BG39" s="31"/>
+      <c r="BH39" s="31"/>
+      <c r="BI39" s="31"/>
+      <c r="BJ39" s="31"/>
+      <c r="BK39" s="31"/>
+      <c r="BL39" s="31"/>
+      <c r="BM39" s="31"/>
+      <c r="BN39" s="31"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
@@ -7585,8 +7893,8 @@
     <mergeCell ref="Y5:AE5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="H30:H36 H9">
-    <cfRule type="dataBar" priority="86">
+  <conditionalFormatting sqref="H32:H38 H9">
+    <cfRule type="dataBar" priority="94">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7600,25 +7908,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:BN7">
-    <cfRule type="expression" dxfId="69" priority="129">
+    <cfRule type="expression" dxfId="75" priority="137">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K9:BN9 K30:BN36">
-    <cfRule type="expression" dxfId="68" priority="132">
+  <conditionalFormatting sqref="K9:BN9 K32:BN38">
+    <cfRule type="expression" dxfId="74" priority="140">
       <formula>AND($E9&lt;=K$6,ROUNDDOWN(($F9-$E9+1)*$H9,0)+$E9-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="133">
+    <cfRule type="expression" dxfId="73" priority="141">
       <formula>AND(NOT(ISBLANK($E9)),$E9&lt;=K$6,$F9&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K6:BN7 K30:BN36 K9:BN9">
-    <cfRule type="expression" dxfId="66" priority="92">
+  <conditionalFormatting sqref="K6:BN7 K32:BN38 K9:BN9">
+    <cfRule type="expression" dxfId="72" priority="100">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="dataBar" priority="81">
+    <cfRule type="dataBar" priority="89">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7632,20 +7940,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15:BN15">
-    <cfRule type="expression" dxfId="65" priority="83">
+    <cfRule type="expression" dxfId="71" priority="91">
       <formula>AND($E15&lt;=K$6,ROUNDDOWN(($F15-$E15+1)*$H15,0)+$E15-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="84">
+    <cfRule type="expression" dxfId="70" priority="92">
       <formula>AND(NOT(ISBLANK($E15)),$E15&lt;=K$6,$F15&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15:BN15">
-    <cfRule type="expression" dxfId="63" priority="82">
+    <cfRule type="expression" dxfId="69" priority="90">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H29">
-    <cfRule type="dataBar" priority="77">
+  <conditionalFormatting sqref="H31">
+    <cfRule type="dataBar" priority="85">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7658,21 +7966,21 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K29:BN29">
-    <cfRule type="expression" dxfId="62" priority="79">
-      <formula>AND($E29&lt;=K$6,ROUNDDOWN(($F29-$E29+1)*$H29,0)+$E29-1&gt;=K$6)</formula>
+  <conditionalFormatting sqref="K31:BN31">
+    <cfRule type="expression" dxfId="68" priority="87">
+      <formula>AND($E31&lt;=K$6,ROUNDDOWN(($F31-$E31+1)*$H31,0)+$E31-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="80">
-      <formula>AND(NOT(ISBLANK($E29)),$E29&lt;=K$6,$F29&gt;=K$6)</formula>
+    <cfRule type="expression" dxfId="67" priority="88">
+      <formula>AND(NOT(ISBLANK($E31)),$E31&lt;=K$6,$F31&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K29:BN29">
-    <cfRule type="expression" dxfId="60" priority="78">
+  <conditionalFormatting sqref="K31:BN31">
+    <cfRule type="expression" dxfId="66" priority="86">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="dataBar" priority="73">
+    <cfRule type="dataBar" priority="81">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7686,20 +7994,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10:BN10">
-    <cfRule type="expression" dxfId="59" priority="75">
+    <cfRule type="expression" dxfId="65" priority="83">
       <formula>AND($E10&lt;=K$6,ROUNDDOWN(($F10-$E10+1)*$H10,0)+$E10-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="76">
+    <cfRule type="expression" dxfId="64" priority="84">
       <formula>AND(NOT(ISBLANK($E10)),$E10&lt;=K$6,$F10&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10:BN10">
-    <cfRule type="expression" dxfId="57" priority="74">
+    <cfRule type="expression" dxfId="63" priority="82">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="dataBar" priority="69">
+    <cfRule type="dataBar" priority="77">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7713,20 +8021,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11:BN11">
-    <cfRule type="expression" dxfId="56" priority="71">
+    <cfRule type="expression" dxfId="62" priority="79">
       <formula>AND($E11&lt;=K$6,ROUNDDOWN(($F11-$E11+1)*$H11,0)+$E11-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="72">
+    <cfRule type="expression" dxfId="61" priority="80">
       <formula>AND(NOT(ISBLANK($E11)),$E11&lt;=K$6,$F11&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11:BN11">
-    <cfRule type="expression" dxfId="54" priority="70">
+    <cfRule type="expression" dxfId="60" priority="78">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14">
-    <cfRule type="dataBar" priority="65">
+    <cfRule type="dataBar" priority="73">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7740,7 +8048,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="dataBar" priority="53">
+    <cfRule type="dataBar" priority="61">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7754,20 +8062,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14:BN14">
-    <cfRule type="expression" dxfId="53" priority="67">
+    <cfRule type="expression" dxfId="59" priority="75">
       <formula>AND($E14&lt;=K$6,ROUNDDOWN(($F14-$E14+1)*$H14,0)+$E14-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="68">
+    <cfRule type="expression" dxfId="58" priority="76">
       <formula>AND(NOT(ISBLANK($E14)),$E14&lt;=K$6,$F14&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14:BN14">
-    <cfRule type="expression" dxfId="51" priority="66">
+    <cfRule type="expression" dxfId="57" priority="74">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="dataBar" priority="61">
+    <cfRule type="dataBar" priority="69">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7781,20 +8089,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16:BN16">
-    <cfRule type="expression" dxfId="50" priority="63">
+    <cfRule type="expression" dxfId="56" priority="71">
       <formula>AND($E16&lt;=K$6,ROUNDDOWN(($F16-$E16+1)*$H16,0)+$E16-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="64">
+    <cfRule type="expression" dxfId="55" priority="72">
       <formula>AND(NOT(ISBLANK($E16)),$E16&lt;=K$6,$F16&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16:BN16">
-    <cfRule type="expression" dxfId="48" priority="62">
+    <cfRule type="expression" dxfId="54" priority="70">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="dataBar" priority="57">
+    <cfRule type="dataBar" priority="65">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7808,20 +8116,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24:BN24">
-    <cfRule type="expression" dxfId="47" priority="59">
+    <cfRule type="expression" dxfId="53" priority="67">
       <formula>AND($E24&lt;=K$6,ROUNDDOWN(($F24-$E24+1)*$H24,0)+$E24-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="60">
+    <cfRule type="expression" dxfId="52" priority="68">
       <formula>AND(NOT(ISBLANK($E24)),$E24&lt;=K$6,$F24&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24:BN24">
-    <cfRule type="expression" dxfId="45" priority="58">
+    <cfRule type="expression" dxfId="51" priority="66">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="dataBar" priority="49">
+    <cfRule type="dataBar" priority="57">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7835,20 +8143,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K25:BN25">
-    <cfRule type="expression" dxfId="44" priority="55">
+    <cfRule type="expression" dxfId="50" priority="63">
       <formula>AND($E25&lt;=K$6,ROUNDDOWN(($F25-$E25+1)*$H25,0)+$E25-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="56">
+    <cfRule type="expression" dxfId="49" priority="64">
       <formula>AND(NOT(ISBLANK($E25)),$E25&lt;=K$6,$F25&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K25:BN25">
-    <cfRule type="expression" dxfId="42" priority="54">
+    <cfRule type="expression" dxfId="48" priority="62">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="dataBar" priority="45">
+    <cfRule type="dataBar" priority="53">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7862,20 +8170,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8:BN8">
-    <cfRule type="expression" dxfId="41" priority="51">
+    <cfRule type="expression" dxfId="47" priority="59">
       <formula>AND($E8&lt;=K$6,ROUNDDOWN(($F8-$E8+1)*$H8,0)+$E8-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="52">
+    <cfRule type="expression" dxfId="46" priority="60">
       <formula>AND(NOT(ISBLANK($E8)),$E8&lt;=K$6,$F8&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8:BN8">
-    <cfRule type="expression" dxfId="39" priority="50">
+    <cfRule type="expression" dxfId="45" priority="58">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18">
-    <cfRule type="dataBar" priority="41">
+    <cfRule type="dataBar" priority="49">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7889,20 +8197,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K17:BN17">
-    <cfRule type="expression" dxfId="38" priority="47">
+    <cfRule type="expression" dxfId="44" priority="55">
       <formula>AND($E17&lt;=K$6,ROUNDDOWN(($F17-$E17+1)*$H17,0)+$E17-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="48">
+    <cfRule type="expression" dxfId="43" priority="56">
       <formula>AND(NOT(ISBLANK($E17)),$E17&lt;=K$6,$F17&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K17:BN17">
-    <cfRule type="expression" dxfId="36" priority="46">
+    <cfRule type="expression" dxfId="42" priority="54">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19">
-    <cfRule type="dataBar" priority="37">
+    <cfRule type="dataBar" priority="45">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7916,20 +8224,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18:BN18">
-    <cfRule type="expression" dxfId="35" priority="43">
+    <cfRule type="expression" dxfId="41" priority="51">
       <formula>AND($E18&lt;=K$6,ROUNDDOWN(($F18-$E18+1)*$H18,0)+$E18-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="44">
+    <cfRule type="expression" dxfId="40" priority="52">
       <formula>AND(NOT(ISBLANK($E18)),$E18&lt;=K$6,$F18&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18:BN18">
-    <cfRule type="expression" dxfId="33" priority="42">
+    <cfRule type="expression" dxfId="39" priority="50">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H20">
-    <cfRule type="dataBar" priority="33">
+    <cfRule type="dataBar" priority="41">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7943,20 +8251,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K19:BN19">
-    <cfRule type="expression" dxfId="32" priority="39">
+    <cfRule type="expression" dxfId="38" priority="47">
       <formula>AND($E19&lt;=K$6,ROUNDDOWN(($F19-$E19+1)*$H19,0)+$E19-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="40">
+    <cfRule type="expression" dxfId="37" priority="48">
       <formula>AND(NOT(ISBLANK($E19)),$E19&lt;=K$6,$F19&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K19:BN19">
-    <cfRule type="expression" dxfId="30" priority="38">
+    <cfRule type="expression" dxfId="36" priority="46">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="dataBar" priority="29">
+    <cfRule type="dataBar" priority="37">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7970,20 +8278,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20:BN20">
-    <cfRule type="expression" dxfId="29" priority="35">
+    <cfRule type="expression" dxfId="35" priority="43">
       <formula>AND($E20&lt;=K$6,ROUNDDOWN(($F20-$E20+1)*$H20,0)+$E20-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="36">
+    <cfRule type="expression" dxfId="34" priority="44">
       <formula>AND(NOT(ISBLANK($E20)),$E20&lt;=K$6,$F20&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20:BN20">
-    <cfRule type="expression" dxfId="27" priority="34">
+    <cfRule type="expression" dxfId="33" priority="42">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="dataBar" priority="25">
+    <cfRule type="dataBar" priority="33">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7997,20 +8305,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21:BN21">
-    <cfRule type="expression" dxfId="26" priority="31">
+    <cfRule type="expression" dxfId="32" priority="39">
       <formula>AND($E21&lt;=K$6,ROUNDDOWN(($F21-$E21+1)*$H21,0)+$E21-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="32">
+    <cfRule type="expression" dxfId="31" priority="40">
       <formula>AND(NOT(ISBLANK($E21)),$E21&lt;=K$6,$F21&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21:BN21">
-    <cfRule type="expression" dxfId="24" priority="30">
+    <cfRule type="expression" dxfId="30" priority="38">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="dataBar" priority="21">
+    <cfRule type="dataBar" priority="29">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8024,20 +8332,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22:BN22">
-    <cfRule type="expression" dxfId="23" priority="27">
+    <cfRule type="expression" dxfId="29" priority="35">
       <formula>AND($E22&lt;=K$6,ROUNDDOWN(($F22-$E22+1)*$H22,0)+$E22-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="28">
+    <cfRule type="expression" dxfId="28" priority="36">
       <formula>AND(NOT(ISBLANK($E22)),$E22&lt;=K$6,$F22&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22:BN22">
-    <cfRule type="expression" dxfId="21" priority="26">
+    <cfRule type="expression" dxfId="27" priority="34">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="dataBar" priority="17">
+    <cfRule type="dataBar" priority="25">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8051,33 +8359,33 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K23:BN23">
-    <cfRule type="expression" dxfId="20" priority="23">
+    <cfRule type="expression" dxfId="26" priority="31">
       <formula>AND($E23&lt;=K$6,ROUNDDOWN(($F23-$E23+1)*$H23,0)+$E23-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="24">
+    <cfRule type="expression" dxfId="25" priority="32">
       <formula>AND(NOT(ISBLANK($E23)),$E23&lt;=K$6,$F23&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K23:BN23">
-    <cfRule type="expression" dxfId="18" priority="22">
+    <cfRule type="expression" dxfId="24" priority="30">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12:BN12">
-    <cfRule type="expression" dxfId="17" priority="19">
+    <cfRule type="expression" dxfId="23" priority="27">
       <formula>AND($E12&lt;=K$6,ROUNDDOWN(($F12-$E12+1)*$H12,0)+$E12-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="20">
+    <cfRule type="expression" dxfId="22" priority="28">
       <formula>AND(NOT(ISBLANK($E12)),$E12&lt;=K$6,$F12&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12:BN12">
-    <cfRule type="expression" dxfId="15" priority="18">
+    <cfRule type="expression" dxfId="21" priority="26">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13">
-    <cfRule type="dataBar" priority="13">
+    <cfRule type="dataBar" priority="21">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8091,20 +8399,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13:BN13">
-    <cfRule type="expression" dxfId="14" priority="15">
+    <cfRule type="expression" dxfId="20" priority="23">
       <formula>AND($E13&lt;=K$6,ROUNDDOWN(($F13-$E13+1)*$H13,0)+$E13-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="16">
+    <cfRule type="expression" dxfId="19" priority="24">
       <formula>AND(NOT(ISBLANK($E13)),$E13&lt;=K$6,$F13&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13:BN13">
-    <cfRule type="expression" dxfId="12" priority="14">
+    <cfRule type="expression" dxfId="18" priority="22">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="dataBar" priority="9">
+    <cfRule type="dataBar" priority="17">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8118,20 +8426,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K26:BN26">
-    <cfRule type="expression" dxfId="11" priority="11">
+    <cfRule type="expression" dxfId="17" priority="19">
       <formula>AND($E26&lt;=K$6,ROUNDDOWN(($F26-$E26+1)*$H26,0)+$E26-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="12">
+    <cfRule type="expression" dxfId="16" priority="20">
       <formula>AND(NOT(ISBLANK($E26)),$E26&lt;=K$6,$F26&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K26:BN26">
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="15" priority="18">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="dataBar" priority="5">
+    <cfRule type="dataBar" priority="13">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8145,20 +8453,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K27:BN27">
-    <cfRule type="expression" dxfId="8" priority="7">
+    <cfRule type="expression" dxfId="14" priority="15">
       <formula>AND($E27&lt;=K$6,ROUNDDOWN(($F27-$E27+1)*$H27,0)+$E27-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="13" priority="16">
       <formula>AND(NOT(ISBLANK($E27)),$E27&lt;=K$6,$F27&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K27:BN27">
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="12" priority="14">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28">
-    <cfRule type="dataBar" priority="1">
+    <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8172,14 +8480,68 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28:BN28">
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="11" priority="11">
       <formula>AND($E28&lt;=K$6,ROUNDDOWN(($F28-$E28+1)*$H28,0)+$E28-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="10" priority="12">
       <formula>AND(NOT(ISBLANK($E28)),$E28&lt;=K$6,$F28&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28:BN28">
+    <cfRule type="expression" dxfId="9" priority="10">
+      <formula>K$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H29">
+    <cfRule type="dataBar" priority="5">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{6D6543B1-9031-4268-81EA-0F0CF2EE0764}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K29:BN29">
+    <cfRule type="expression" dxfId="8" priority="7">
+      <formula>AND($E29&lt;=K$6,ROUNDDOWN(($F29-$E29+1)*$H29,0)+$E29-1&gt;=K$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>AND(NOT(ISBLANK($E29)),$E29&lt;=K$6,$F29&gt;=K$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K29:BN29">
+    <cfRule type="expression" dxfId="6" priority="6">
+      <formula>K$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H30">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{1C1ECBE2-8780-45C7-A4C6-403DB0B3A581}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K30:BN30">
+    <cfRule type="expression" dxfId="5" priority="3">
+      <formula>AND($E30&lt;=K$6,ROUNDDOWN(($F30-$E30+1)*$H30,0)+$E30-1&gt;=K$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="4">
+      <formula>AND(NOT(ISBLANK($E30)),$E30&lt;=K$6,$F30&gt;=K$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K30:BN30">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>K$6=TODAY()</formula>
     </cfRule>
@@ -8194,7 +8556,7 @@
   <pageSetup scale="63" fitToHeight="0" orientation="landscape" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
-    <ignoredError sqref="A30:B30 A32:B32 B31 E30:H32 G33 G34:G35 G36" unlockedFormula="1"/>
+    <ignoredError sqref="A32:B32 A34:B34 B33 E32:H34 G35 G36:G37 G38" unlockedFormula="1"/>
   </ignoredErrors>
   <drawing r:id="rId3"/>
   <legacyDrawing r:id="rId4"/>
@@ -8242,7 +8604,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H30:H36 H9</xm:sqref>
+          <xm:sqref>H32:H38 H9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{07AD01F1-646A-4A0F-A874-0BFB6496601A}">
@@ -8272,7 +8634,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H29</xm:sqref>
+          <xm:sqref>H31</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{58817D81-44C9-4F08-A393-81628B862816}">
@@ -8559,6 +8921,36 @@
           </x14:cfRule>
           <xm:sqref>H28</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{6D6543B1-9031-4268-81EA-0F0CF2EE0764}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H29</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{1C1ECBE2-8780-45C7-A4C6-403DB0B3A581}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H30</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>